<commit_message>
reset of model and included trans files outcomment in IND
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_SUP_ImportExport.xlsx
+++ b/SubRES_TMPL/SubRes_SUP_ImportExport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES models\TIMES-tom\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES Modeller\TIMES-TOM\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B39F236-AA84-45CA-8521-1251E5164E54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCDD3D64-3612-46AB-8267-2EA8B09B9760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19968" yWindow="1200" windowWidth="21000" windowHeight="14220" tabRatio="596" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8145" yWindow="5325" windowWidth="28800" windowHeight="15435" tabRatio="596" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOG" sheetId="7" r:id="rId1"/>
@@ -7356,16 +7356,16 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" customWidth="1"/>
-    <col min="2" max="2" width="15.77734375" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" customWidth="1"/>
-    <col min="4" max="4" width="19.88671875" customWidth="1"/>
-    <col min="5" max="5" width="60.21875" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" customWidth="1"/>
+    <col min="5" max="5" width="60.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>25</v>
       </c>
@@ -7382,7 +7382,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="19">
         <v>42788</v>
       </c>
@@ -7400,7 +7400,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="19">
         <v>42499</v>
       </c>
@@ -7414,7 +7414,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="19">
         <v>42242</v>
       </c>
@@ -7432,7 +7432,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="19">
         <v>42233</v>
       </c>
@@ -7467,20 +7467,20 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="28"/>
+    <col min="1" max="1" width="9.140625" style="28"/>
     <col min="2" max="2" width="24" style="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="138.44140625" style="28" customWidth="1"/>
-    <col min="4" max="16384" width="9.109375" style="28"/>
+    <col min="3" max="3" width="138.42578125" style="28" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="27" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B3" s="29" t="s">
         <v>39</v>
       </c>
@@ -7488,24 +7488,24 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B4" s="29" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B5" s="29"/>
     </row>
-    <row r="6" spans="2:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="29"/>
     </row>
-    <row r="7" spans="2:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B7" s="29"/>
     </row>
-    <row r="8" spans="2:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="29"/>
     </row>
-    <row r="9" spans="2:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="29" t="s">
         <v>41</v>
       </c>
@@ -7513,18 +7513,18 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B10" s="29"/>
     </row>
-    <row r="11" spans="2:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" s="30" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" s="29"/>
     </row>
-    <row r="13" spans="2:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B13" s="31" t="s">
         <v>31</v>
       </c>
@@ -7551,27 +7551,27 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A2:J59"/>
+  <dimension ref="A2:N59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.21875" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.21875" customWidth="1"/>
-    <col min="9" max="9" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="26" t="s">
@@ -7579,7 +7579,7 @@
       </c>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:10" s="6" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" s="6" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="C3" s="22" t="s">
         <v>2</v>
@@ -7603,7 +7603,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="7" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" s="7" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="C4" s="21" t="s">
         <v>33</v>
@@ -7627,7 +7627,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="C5" s="33" t="s">
         <v>67</v>
@@ -7646,7 +7646,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="C6" s="33" t="s">
         <v>68</v>
@@ -7665,7 +7665,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="C7" s="33" t="s">
         <v>69</v>
@@ -7683,8 +7683,11 @@
       <c r="H7" s="16">
         <v>0.95</v>
       </c>
+      <c r="N7" s="1">
+        <v>1</v>
+      </c>
     </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="C8" s="33" t="s">
         <v>70</v>
@@ -7703,7 +7706,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="C9" s="33" t="s">
         <v>72</v>
@@ -7722,7 +7725,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="C10" s="33" t="s">
         <v>73</v>
@@ -7741,7 +7744,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="C11" s="33" t="s">
         <v>74</v>
@@ -7760,7 +7763,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="C12" s="33" t="s">
         <v>75</v>
@@ -7779,7 +7782,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="C13" s="33" t="s">
         <v>76</v>
@@ -7798,7 +7801,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="C14" s="33" t="s">
         <v>77</v>
@@ -7817,7 +7820,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="C15" s="33" t="s">
         <v>78</v>
@@ -7835,11 +7838,11 @@
       <c r="H15" s="16">
         <v>0.95</v>
       </c>
-      <c r="J15" s="33" t="s">
+      <c r="M15" s="33" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="C16" s="33" t="s">
         <v>79</v>
@@ -7857,11 +7860,11 @@
       <c r="H16" s="16">
         <v>0.95</v>
       </c>
-      <c r="J16" s="33" t="s">
+      <c r="M16" s="33" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="C17" s="33" t="s">
         <v>80</v>
@@ -7879,11 +7882,11 @@
       <c r="H17" s="16">
         <v>0.95</v>
       </c>
-      <c r="J17" s="33" t="s">
+      <c r="M17" s="33" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="C18" s="33" t="s">
         <v>81</v>
@@ -7901,101 +7904,101 @@
       <c r="H18" s="16">
         <v>0.95</v>
       </c>
-      <c r="J18" s="33" t="s">
+      <c r="M18" s="33" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:10" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
-      <c r="J19" s="33" t="s">
+      <c r="M19" s="33" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:10" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
-      <c r="J20" s="33" t="s">
+      <c r="M20" s="33" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
-      <c r="J21" s="33" t="s">
+      <c r="M21" s="33" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:10" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
-      <c r="J22" s="33" t="s">
+      <c r="M22" s="33" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:10" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
-      <c r="J23" s="33" t="s">
+      <c r="M23" s="33" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:10" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
-      <c r="J24" s="33" t="s">
+      <c r="M24" s="33" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:10" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
-      <c r="J25" s="33" t="s">
+      <c r="M25" s="33" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:10" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
-      <c r="J26" s="33" t="s">
+      <c r="M26" s="33" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:10" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
-      <c r="J27" s="33" t="s">
+      <c r="M27" s="33" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:10" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
-      <c r="J28" s="33" t="s">
+      <c r="M28" s="33" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I30" s="8"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I31" s="8"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I32" s="8"/>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
       <c r="I33" s="8"/>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
       <c r="I34" s="8"/>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
       <c r="I35" s="8"/>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
       <c r="I36" s="8"/>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.2">
       <c r="I37" s="8"/>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
       <c r="I38" s="8"/>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B43" s="9" t="s">
         <v>0</v>
       </c>
@@ -8007,7 +8010,7 @@
       <c r="H43" s="10"/>
       <c r="I43" s="10"/>
     </row>
-    <row r="44" spans="2:9" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B44" s="11" t="s">
         <v>1</v>
       </c>
@@ -8033,7 +8036,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="2:9" ht="31.2" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:9" ht="34.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B45" s="12" t="s">
         <v>9</v>
       </c>
@@ -8059,7 +8062,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B46" s="14" t="s">
         <v>23</v>
       </c>
@@ -8079,7 +8082,7 @@
       <c r="H46" s="10"/>
       <c r="I46" s="10"/>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B47" s="2"/>
       <c r="C47" s="33" t="s">
         <v>68</v>
@@ -8097,7 +8100,7 @@
       <c r="H47" s="10"/>
       <c r="I47" s="10"/>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B48" s="2"/>
       <c r="C48" s="33" t="s">
         <v>69</v>
@@ -8115,7 +8118,7 @@
       <c r="H48" s="10"/>
       <c r="I48" s="10"/>
     </row>
-    <row r="49" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C49" s="33" t="s">
         <v>70</v>
       </c>
@@ -8131,7 +8134,7 @@
       <c r="H49" s="10"/>
       <c r="I49" s="10"/>
     </row>
-    <row r="50" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C50" s="33" t="s">
         <v>72</v>
       </c>
@@ -8147,7 +8150,7 @@
       <c r="H50" s="10"/>
       <c r="I50" s="10"/>
     </row>
-    <row r="51" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C51" s="33" t="s">
         <v>73</v>
       </c>
@@ -8163,7 +8166,7 @@
       <c r="H51" s="10"/>
       <c r="I51" s="10"/>
     </row>
-    <row r="52" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C52" s="33" t="s">
         <v>74</v>
       </c>
@@ -8179,7 +8182,7 @@
       <c r="H52" s="10"/>
       <c r="I52" s="10"/>
     </row>
-    <row r="53" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C53" s="33" t="s">
         <v>75</v>
       </c>
@@ -8195,7 +8198,7 @@
       <c r="H53" s="10"/>
       <c r="I53" s="10"/>
     </row>
-    <row r="54" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C54" s="33" t="s">
         <v>76</v>
       </c>
@@ -8211,7 +8214,7 @@
       <c r="H54" s="10"/>
       <c r="I54" s="10"/>
     </row>
-    <row r="55" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C55" s="33" t="s">
         <v>77</v>
       </c>
@@ -8227,7 +8230,7 @@
       <c r="H55" s="10"/>
       <c r="I55" s="10"/>
     </row>
-    <row r="56" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C56" s="33" t="s">
         <v>78</v>
       </c>
@@ -8241,7 +8244,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="57" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C57" s="33" t="s">
         <v>79</v>
       </c>
@@ -8255,7 +8258,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="58" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C58" s="33" t="s">
         <v>80</v>
       </c>
@@ -8269,7 +8272,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="59" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C59" s="33" t="s">
         <v>81</v>
       </c>

</xml_diff>